<commit_message>
Healthy status added to experimental data
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Ducry1979.xlsx
+++ b/experimental_data/GEC/Ducry1979.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="193" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="193" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Ducry1979" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
     <t>subject</t>
   </si>
   <si>
-    <t>state</t>
+    <t>status</t>
   </si>
   <si>
     <t>trained</t>
@@ -116,7 +116,7 @@
     <t>H.R.</t>
   </si>
   <si>
-    <t>normal</t>
+    <t>healthy</t>
   </si>
   <si>
     <t>G.F.</t>
@@ -169,8 +169,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -235,7 +235,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -244,79 +244,79 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -382,23 +382,23 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>277560</xdr:colOff>
+      <xdr:colOff>304560</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>582480</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:colOff>609120</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="" id="0" name="Graphics 1"/>
+        <xdr:cNvPr id="0" name="Graphics 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -409,8 +409,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="277560" y="3349800"/>
-          <a:ext cx="6202080" cy="3629880"/>
+          <a:off x="304560" y="3340800"/>
+          <a:ext cx="6201720" cy="3629520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -432,8 +432,8 @@
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6:B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -442,7 +442,7 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,13 +452,13 @@
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="3" s="5">
+    <row r="3" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -508,7 +508,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>30</v>
       </c>
@@ -610,7 +610,7 @@
         <v>0.0433333333333333</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>30</v>
       </c>
@@ -662,7 +662,7 @@
         <v>0.0383333333333333</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>30</v>
       </c>
@@ -714,7 +714,7 @@
         <v>0.0344444444444444</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>30</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.0333333333333333</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
@@ -818,7 +818,7 @@
         <v>0.0411111111111111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
@@ -870,7 +870,7 @@
         <v>0.0555555555555556</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
@@ -922,7 +922,7 @@
         <v>0.0355555555555556</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>30</v>
       </c>
@@ -972,7 +972,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>30</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>0.045</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>30</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>0.0338888888888889</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>30</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>0.0433333333333333</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>30</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>0.0361111111111111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>30</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0.0366666666666667</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>30</v>
       </c>
@@ -1287,7 +1287,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>